<commit_message>
Mejora reporte trazabilidad pcl pbs 088 y Implementacion pbs 090 parte 1
</commit_message>
<xml_diff>
--- a/public/Plantilla_Reporte_Trazabilidad_Pcl/plantilla_repor_traza_pcl.xlsx
+++ b/public/Plantilla_Reporte_Trazabilidad_Pcl/plantilla_repor_traza_pcl.xlsx
@@ -418,7 +418,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -457,6 +457,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,9 +702,9 @@
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" style="5" customWidth="1"/>
     <col min="8" max="8" width="38.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="14" customWidth="1"/>
     <col min="10" max="10" width="50.140625" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="11" max="11" width="16" style="14" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" customWidth="1"/>

</xml_diff>